<commit_message>
ADD: add S3 code
</commit_message>
<xml_diff>
--- a/instance_info_backend.xlsx
+++ b/instance_info_backend.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,6 +561,33 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>i-06f0711b81a89db89</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>t2.micro</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>172.31.11.26</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2023-11-17 08:54:32+00:00</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>launch-wizard-2</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>